<commit_message>
ATEENDIGO - 7(Revisi) + 11 - 15
</commit_message>
<xml_diff>
--- a/Excel/2. Esign.xlsx
+++ b/Excel/2. Esign.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="109">
   <si>
     <t>Status</t>
   </si>
@@ -329,13 +329,64 @@
     <t>confins</t>
   </si>
   <si>
-    <t>7777777777777777</t>
-  </si>
-  <si>
-    <t>deny</t>
-  </si>
-  <si>
-    <t>08274827384972</t>
+    <t>2733849283748273</t>
+  </si>
+  <si>
+    <t>jakarta</t>
+  </si>
+  <si>
+    <t>02/20/2000</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>jl kemang</t>
+  </si>
+  <si>
+    <t>jakarta barat</t>
+  </si>
+  <si>
+    <t>kebon</t>
+  </si>
+  <si>
+    <t>jeruk</t>
+  </si>
+  <si>
+    <t>apel</t>
+  </si>
+  <si>
+    <t>Inquiry Invitation Action</t>
+  </si>
+  <si>
+    <t>fen@gmail.com</t>
+  </si>
+  <si>
+    <t>Daftar Akun</t>
+  </si>
+  <si>
+    <t>Edit Invitation Inquiry</t>
+  </si>
+  <si>
+    <t>Invite By</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>fen</t>
+  </si>
+  <si>
+    <t>Input with</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Resend</t>
+  </si>
+  <si>
+    <t>081220380088</t>
   </si>
 </sst>
 </file>
@@ -469,7 +520,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -509,6 +560,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -792,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -808,7 +860,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="1"/>
@@ -819,7 +871,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1"/>
@@ -855,15 +907,23 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -893,7 +953,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -903,7 +963,9 @@
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -912,7 +974,9 @@
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -921,7 +985,9 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -931,7 +997,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -941,7 +1007,9 @@
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -959,7 +1027,9 @@
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -968,7 +1038,9 @@
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -977,7 +1049,9 @@
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -986,7 +1060,9 @@
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -995,7 +1071,9 @@
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1004,7 +1082,9 @@
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>12862</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1013,7 +1093,9 @@
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1055,7 +1137,9 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="11"/>
+      <c r="A28" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -1074,14 +1158,41 @@
         <v>26</v>
       </c>
     </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
       <formula1>"M, F"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>"Phone, Id no, Email"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"Edit, Resend"</formula1>
+    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1089,16 +1200,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="25" style="30" customWidth="1"/>
-    <col min="3" max="6" width="21" style="30" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="24.42578125" style="30" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" style="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" style="30" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="21" style="30" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="14" customFormat="1">

</xml_diff>

<commit_message>
ATEENDIGO - 32 + 33 + 34 + 35
</commit_message>
<xml_diff>
--- a/Excel/2. Esign.xlsx
+++ b/Excel/2. Esign.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\Katalon Studio\ATeSign\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7065" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="7065" windowWidth="18525" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BuatUndangan" sheetId="2" r:id="rId1"/>
-    <sheet name="API Send Document" sheetId="4" r:id="rId2"/>
-    <sheet name="API Generate Inv Link" sheetId="6" r:id="rId3"/>
-    <sheet name="PencarianPengguna" sheetId="7" r:id="rId4"/>
+    <sheet name="BuatUndangan" r:id="rId1" sheetId="2"/>
+    <sheet name="API Send Document" r:id="rId2" sheetId="4"/>
+    <sheet name="API Generate Inv Link" r:id="rId3" sheetId="6"/>
+    <sheet name="PencarianPengguna" r:id="rId4" sheetId="7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -27,7 +27,7 @@
     <author>Fendy Tio</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
     <author>Fendy Tio</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="255">
   <si>
     <t>Status</t>
   </si>
@@ -858,13 +858,14 @@
     <t>$Email</t>
   </si>
   <si>
-    <t>Edit</t>
+    <t>Resend Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1006,76 +1007,76 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="14" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="2"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1092,10 +1093,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1259,21 +1260,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1290,7 +1291,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1344,8 +1345,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -1353,8 +1354,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1701,32 +1702,32 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B32" type="list">
       <formula1>"SMS, Email"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
       <formula1>"Edit, Resend"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7" type="list">
       <formula1>"Phone, Id no, Email"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B13" type="list">
       <formula1>"M, F"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" tooltip="mailto:wikiy.hendraa@ad-ins.com"/>
-    <hyperlink ref="B33" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="B15" tooltip="mailto:wikiy.hendraa@ad-ins.com"/>
+    <hyperlink r:id="rId2" ref="B33"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
@@ -1734,26 +1735,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="19" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="63" style="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.28515625" style="19" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="21" style="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" style="19" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.7109375" style="19" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.42578125" style="19" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.28515625" style="19" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.7109375" style="19" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.42578125" style="19" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="25.85546875" style="19" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.28515625" style="19" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.140625" style="19" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.28515625" style="19" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="27" style="19" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.7109375" style="19" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9" style="19" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="19" width="24.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="19" width="63.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="19" width="39.28515625" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" style="19" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="19" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="19" width="20.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="19" width="20.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="19" width="21.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="19" width="21.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="19" width="20.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="19" width="25.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="19" width="24.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="19" width="17.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="19" width="19.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="19" width="27.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="19" width="21.7109375" collapsed="true"/>
+    <col min="19" max="16384" style="19" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="1" s="13" spans="1:18">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="2" s="13" spans="1:18">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1865,13 +1866,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="3" s="13" spans="1:18">
       <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="4" s="13" spans="1:18">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -1880,59 +1881,59 @@
         <v>0</v>
       </c>
       <c r="C4" s="14">
-        <f t="shared" ref="C4:P4" si="0">COUNTIFS($A9:$A47,"*$*",C9:C47,"")</f>
+        <f ref="C4:P4" si="0" t="shared">COUNTIFS($A9:$A47,"*$*",C9:C47,"")</f>
         <v>0</v>
       </c>
       <c r="D4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4" s="14">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4" s="14">
@@ -1940,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="5" s="13" spans="1:18">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1957,7 +1958,7 @@
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
     </row>
-    <row r="6" spans="1:18" s="14" customFormat="1" ht="90">
+    <row customFormat="1" ht="90" r="6" s="14" spans="1:18">
       <c r="A6" s="20" t="s">
         <v>67</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="7" s="13" spans="1:18">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -2033,7 +2034,7 @@
       <c r="Q7" s="21"/>
       <c r="R7" s="21"/>
     </row>
-    <row r="8" spans="1:18" s="15" customFormat="1">
+    <row customFormat="1" r="8" s="15" spans="1:18">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24"/>
@@ -2053,7 +2054,7 @@
       <c r="Q8" s="23"/>
       <c r="R8" s="23"/>
     </row>
-    <row r="9" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="9" s="13" spans="1:18">
       <c r="A9" s="25" t="s">
         <v>85</v>
       </c>
@@ -2109,7 +2110,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="16" customFormat="1">
+    <row customFormat="1" r="10" s="16" spans="1:18">
       <c r="A10" s="26" t="s">
         <v>89</v>
       </c>
@@ -2131,7 +2132,7 @@
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
     </row>
-    <row r="11" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="11" s="13" spans="1:18">
       <c r="A11" s="25" t="s">
         <v>90</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="12" s="13" spans="1:18">
       <c r="A12" s="25" t="s">
         <v>106</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="13" s="13" spans="1:18">
       <c r="A13" s="25" t="s">
         <v>107</v>
       </c>
@@ -2299,7 +2300,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="14" s="13" spans="1:18">
       <c r="A14" s="25" t="s">
         <v>111</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="15" s="13" spans="1:18">
       <c r="A15" s="25" t="s">
         <v>113</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="16" s="13" spans="1:18">
       <c r="A16" s="25" t="s">
         <v>115</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="17" s="13" spans="1:18">
       <c r="A17" s="25" t="s">
         <v>118</v>
       </c>
@@ -2523,7 +2524,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="18" s="13" spans="1:18">
       <c r="A18" s="25" t="s">
         <v>121</v>
       </c>
@@ -2579,7 +2580,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="19" s="13" spans="1:18">
       <c r="A19" s="25" t="s">
         <v>123</v>
       </c>
@@ -2635,7 +2636,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="20" s="13" spans="1:18">
       <c r="A20" s="25" t="s">
         <v>125</v>
       </c>
@@ -2691,7 +2692,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="21" s="13" spans="1:18">
       <c r="A21" s="25" t="s">
         <v>126</v>
       </c>
@@ -2747,7 +2748,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="22" s="13" spans="1:18">
       <c r="A22" s="25" t="s">
         <v>128</v>
       </c>
@@ -2803,7 +2804,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="23" s="13" spans="1:18">
       <c r="A23" s="25" t="s">
         <v>129</v>
       </c>
@@ -2859,7 +2860,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="24" s="13" spans="1:18">
       <c r="A24" s="25" t="s">
         <v>132</v>
       </c>
@@ -2915,7 +2916,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="25" s="13" spans="1:18">
       <c r="A25" s="25" t="s">
         <v>134</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="17" customFormat="1">
+    <row customFormat="1" r="26" s="17" spans="1:18">
       <c r="A26" s="26" t="s">
         <v>136</v>
       </c>
@@ -2993,7 +2994,7 @@
       <c r="Q26" s="26"/>
       <c r="R26" s="26"/>
     </row>
-    <row r="27" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="27" s="13" spans="1:18">
       <c r="A27" s="25" t="s">
         <v>137</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="28" s="13" spans="1:18">
       <c r="A28" s="25" t="s">
         <v>142</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="29" s="13" spans="1:18">
       <c r="A29" s="25" t="s">
         <v>148</v>
       </c>
@@ -3161,7 +3162,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="30" s="13" spans="1:18">
       <c r="A30" s="25" t="s">
         <v>152</v>
       </c>
@@ -3217,7 +3218,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="31" s="13" spans="1:18">
       <c r="A31" s="25" t="s">
         <v>170</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="32" s="13" spans="1:18">
       <c r="A32" s="25" t="s">
         <v>31</v>
       </c>
@@ -3329,7 +3330,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="33" s="13" spans="1:18">
       <c r="A33" s="25" t="s">
         <v>33</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="34" s="13" spans="1:18">
       <c r="A34" s="25" t="s">
         <v>180</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="35" s="13" spans="1:18">
       <c r="A35" s="25" t="s">
         <v>29</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="36" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="36" s="13" spans="1:18">
       <c r="A36" s="25" t="s">
         <v>187</v>
       </c>
@@ -3553,7 +3554,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="37" s="13" spans="1:18">
       <c r="A37" s="25" t="s">
         <v>191</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="38" s="13" spans="1:18">
       <c r="A38" s="25" t="s">
         <v>197</v>
       </c>
@@ -3665,7 +3666,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="39" s="13" spans="1:18">
       <c r="A39" s="25" t="s">
         <v>27</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="40" s="13" spans="1:18">
       <c r="A40" s="25" t="s">
         <v>204</v>
       </c>
@@ -3777,7 +3778,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="41" s="13" spans="1:18">
       <c r="A41" s="25" t="s">
         <v>209</v>
       </c>
@@ -3833,7 +3834,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="42" s="13" spans="1:18">
       <c r="A42" s="25" t="s">
         <v>210</v>
       </c>
@@ -3889,7 +3890,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="43" s="13" spans="1:18">
       <c r="A43" s="25" t="s">
         <v>216</v>
       </c>
@@ -3945,7 +3946,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="44" s="13" spans="1:18">
       <c r="A44" s="25" t="s">
         <v>220</v>
       </c>
@@ -4001,7 +4002,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="45" s="13" spans="1:18">
       <c r="A45" s="25" t="s">
         <v>221</v>
       </c>
@@ -4057,7 +4058,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:18" s="18" customFormat="1">
+    <row customFormat="1" r="46" s="18" spans="1:18">
       <c r="A46" s="33" t="s">
         <v>222</v>
       </c>
@@ -4079,7 +4080,7 @@
       <c r="Q46" s="34"/>
       <c r="R46" s="34"/>
     </row>
-    <row r="47" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="47" s="13" spans="1:18">
       <c r="A47" s="25" t="s">
         <v>223</v>
       </c>
@@ -4135,7 +4136,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:18" s="13" customFormat="1">
+    <row customFormat="1" r="48" s="13" spans="1:18">
       <c r="A48" s="25"/>
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
@@ -4153,77 +4154,77 @@
       <c r="O48" s="25"/>
       <c r="P48" s="25"/>
     </row>
-    <row r="49" spans="2:8" s="13" customFormat="1">
+    <row customFormat="1" r="49" s="13" spans="2:8">
       <c r="B49" s="20"/>
       <c r="C49" s="14"/>
       <c r="H49" s="25"/>
     </row>
-    <row r="50" spans="2:8" ht="29.1" customHeight="1">
+    <row customHeight="1" ht="29.1" r="50" spans="2:8">
       <c r="B50" s="20"/>
       <c r="C50" s="35"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1"/>
-    <hyperlink ref="B25" r:id="rId2"/>
-    <hyperlink ref="B42" r:id="rId3"/>
-    <hyperlink ref="C24" r:id="rId4"/>
-    <hyperlink ref="C25" r:id="rId5"/>
-    <hyperlink ref="C42" r:id="rId6"/>
-    <hyperlink ref="D24" r:id="rId7"/>
-    <hyperlink ref="D25" r:id="rId8"/>
-    <hyperlink ref="D42" r:id="rId9"/>
-    <hyperlink ref="E24" r:id="rId10"/>
-    <hyperlink ref="E25" r:id="rId11"/>
-    <hyperlink ref="E42" r:id="rId12"/>
-    <hyperlink ref="F24" r:id="rId13"/>
-    <hyperlink ref="F25" r:id="rId14"/>
-    <hyperlink ref="F42" r:id="rId15"/>
-    <hyperlink ref="I24" r:id="rId16"/>
-    <hyperlink ref="I25" r:id="rId17"/>
-    <hyperlink ref="I42" r:id="rId18"/>
-    <hyperlink ref="J24" r:id="rId19"/>
-    <hyperlink ref="J25" r:id="rId20"/>
-    <hyperlink ref="J42" r:id="rId21"/>
-    <hyperlink ref="K24" r:id="rId22"/>
-    <hyperlink ref="K25" r:id="rId23"/>
-    <hyperlink ref="K42" r:id="rId24"/>
-    <hyperlink ref="L24" r:id="rId25"/>
-    <hyperlink ref="L25" r:id="rId26"/>
-    <hyperlink ref="L42" r:id="rId27"/>
-    <hyperlink ref="M24" r:id="rId28"/>
-    <hyperlink ref="M25" r:id="rId29"/>
-    <hyperlink ref="M42" r:id="rId30"/>
-    <hyperlink ref="G24" r:id="rId31"/>
-    <hyperlink ref="G25" r:id="rId32"/>
-    <hyperlink ref="G42" r:id="rId33"/>
-    <hyperlink ref="H24" r:id="rId34"/>
-    <hyperlink ref="H25" r:id="rId35"/>
-    <hyperlink ref="H42" r:id="rId36"/>
-    <hyperlink ref="N24" r:id="rId37"/>
-    <hyperlink ref="N25" r:id="rId38"/>
-    <hyperlink ref="N42" r:id="rId39"/>
-    <hyperlink ref="O24" r:id="rId40"/>
-    <hyperlink ref="O25" r:id="rId41"/>
-    <hyperlink ref="O42" r:id="rId42"/>
-    <hyperlink ref="P24" r:id="rId43"/>
-    <hyperlink ref="P25" r:id="rId44"/>
-    <hyperlink ref="P42" r:id="rId45"/>
-    <hyperlink ref="Q24" r:id="rId46"/>
-    <hyperlink ref="Q25" r:id="rId47"/>
-    <hyperlink ref="Q42" r:id="rId48"/>
-    <hyperlink ref="R24" r:id="rId49"/>
-    <hyperlink ref="R25" r:id="rId50"/>
-    <hyperlink ref="R42" r:id="rId51"/>
+    <hyperlink r:id="rId1" ref="B24"/>
+    <hyperlink r:id="rId2" ref="B25"/>
+    <hyperlink r:id="rId3" ref="B42"/>
+    <hyperlink r:id="rId4" ref="C24"/>
+    <hyperlink r:id="rId5" ref="C25"/>
+    <hyperlink r:id="rId6" ref="C42"/>
+    <hyperlink r:id="rId7" ref="D24"/>
+    <hyperlink r:id="rId8" ref="D25"/>
+    <hyperlink r:id="rId9" ref="D42"/>
+    <hyperlink r:id="rId10" ref="E24"/>
+    <hyperlink r:id="rId11" ref="E25"/>
+    <hyperlink r:id="rId12" ref="E42"/>
+    <hyperlink r:id="rId13" ref="F24"/>
+    <hyperlink r:id="rId14" ref="F25"/>
+    <hyperlink r:id="rId15" ref="F42"/>
+    <hyperlink r:id="rId16" ref="I24"/>
+    <hyperlink r:id="rId17" ref="I25"/>
+    <hyperlink r:id="rId18" ref="I42"/>
+    <hyperlink r:id="rId19" ref="J24"/>
+    <hyperlink r:id="rId20" ref="J25"/>
+    <hyperlink r:id="rId21" ref="J42"/>
+    <hyperlink r:id="rId22" ref="K24"/>
+    <hyperlink r:id="rId23" ref="K25"/>
+    <hyperlink r:id="rId24" ref="K42"/>
+    <hyperlink r:id="rId25" ref="L24"/>
+    <hyperlink r:id="rId26" ref="L25"/>
+    <hyperlink r:id="rId27" ref="L42"/>
+    <hyperlink r:id="rId28" ref="M24"/>
+    <hyperlink r:id="rId29" ref="M25"/>
+    <hyperlink r:id="rId30" ref="M42"/>
+    <hyperlink r:id="rId31" ref="G24"/>
+    <hyperlink r:id="rId32" ref="G25"/>
+    <hyperlink r:id="rId33" ref="G42"/>
+    <hyperlink r:id="rId34" ref="H24"/>
+    <hyperlink r:id="rId35" ref="H25"/>
+    <hyperlink r:id="rId36" ref="H42"/>
+    <hyperlink r:id="rId37" ref="N24"/>
+    <hyperlink r:id="rId38" ref="N25"/>
+    <hyperlink r:id="rId39" ref="N42"/>
+    <hyperlink r:id="rId40" ref="O24"/>
+    <hyperlink r:id="rId41" ref="O25"/>
+    <hyperlink r:id="rId42" ref="O42"/>
+    <hyperlink r:id="rId43" ref="P24"/>
+    <hyperlink r:id="rId44" ref="P25"/>
+    <hyperlink r:id="rId45" ref="P42"/>
+    <hyperlink r:id="rId46" ref="Q24"/>
+    <hyperlink r:id="rId47" ref="Q25"/>
+    <hyperlink r:id="rId48" ref="Q42"/>
+    <hyperlink r:id="rId49" ref="R24"/>
+    <hyperlink r:id="rId50" ref="R25"/>
+    <hyperlink r:id="rId51" ref="R42"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -4231,12 +4232,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4328,7 +4329,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="45">
+    <row customFormat="1" ht="45" r="7" s="1" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>225</v>
       </c>
@@ -4348,7 +4349,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1">
+    <row customFormat="1" r="8" s="2" spans="1:6">
       <c r="A8" s="5" t="s">
         <v>231</v>
       </c>
@@ -4370,7 +4371,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1">
+    <row customFormat="1" r="10" s="2" spans="1:6">
       <c r="A10" s="5" t="s">
         <v>233</v>
       </c>
@@ -4392,7 +4393,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1">
+    <row customFormat="1" r="12" s="2" spans="1:6">
       <c r="A12" s="5" t="s">
         <v>234</v>
       </c>
@@ -4658,34 +4659,34 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B38" type="list">
       <formula1>"SMS, Email"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
       <formula1>"Edit, Resend"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 C16">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16 C16" type="list">
       <formula1>"""M"",""F"","""""</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4693,7 +4694,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4806,15 +4807,15 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7" type="list">
       <formula1>"Phone, Id no, Email"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"Edit, Resend"</formula1>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
+      <formula1>"Edit, Resend OTP, Resend Link"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 

</xml_diff>